<commit_message>
More work on planning spreadsheet
</commit_message>
<xml_diff>
--- a/Progress Reports/CDC Monthly progress reports/2017/CDC RIF plans - April 2017 to December 2017.xlsx
+++ b/Progress Reports/CDC Monthly progress reports/2017/CDC RIF plans - April 2017 to December 2017.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>PH</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Background tile download (csache support)</t>
+  </si>
+  <si>
+    <t>Not yet allocated (fault fixing)</t>
   </si>
 </sst>
 </file>
@@ -172,7 +175,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -240,6 +243,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -589,11 +604,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,14 +648,14 @@
         <v>14</v>
       </c>
       <c r="B3" s="11">
-        <f t="shared" ref="B3:B21" si="0">DATE(2017,1,-2)-WEEKDAY(DATE(2017,1,3))+A3*7</f>
+        <f t="shared" ref="B3:B41" si="0">DATE(2017,1,-2)-WEEKDAY(DATE(2017,1,3))+A3*7</f>
         <v>42828</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="20" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="25" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="19" t="s">
@@ -655,9 +670,9 @@
         <f t="shared" si="0"/>
         <v>42835</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
@@ -670,11 +685,11 @@
         <f t="shared" si="0"/>
         <v>42842</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -685,9 +700,9 @@
         <f t="shared" si="0"/>
         <v>42849</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
       <c r="F6" s="14" t="s">
         <v>10</v>
       </c>
@@ -703,10 +718,10 @@
       <c r="C7" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="22"/>
+      <c r="E7" s="26"/>
       <c r="F7" s="18" t="s">
         <v>19</v>
       </c>
@@ -719,13 +734,13 @@
         <f t="shared" si="0"/>
         <v>42863</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="20"/>
+      <c r="E8" s="25"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -736,9 +751,9 @@
         <f t="shared" si="0"/>
         <v>42870</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -749,10 +764,10 @@
         <f t="shared" si="0"/>
         <v>42877</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="25" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="7"/>
@@ -766,8 +781,8 @@
         <f t="shared" si="0"/>
         <v>42884</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="20"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="25"/>
       <c r="E11" s="7"/>
       <c r="F11" s="14"/>
     </row>
@@ -779,8 +794,8 @@
         <f t="shared" si="0"/>
         <v>42891</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="20"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="7"/>
       <c r="F12" s="14"/>
     </row>
@@ -792,14 +807,12 @@
         <f t="shared" si="0"/>
         <v>42898</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>13</v>
+      <c r="C13" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="22" t="s">
+        <v>22</v>
       </c>
       <c r="F13" s="14"/>
     </row>
@@ -811,12 +824,8 @@
         <f t="shared" si="0"/>
         <v>42905</v>
       </c>
-      <c r="C14" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>14</v>
-      </c>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="7"/>
       <c r="F14" s="14"/>
     </row>
@@ -828,8 +837,8 @@
         <f t="shared" si="0"/>
         <v>42912</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
       <c r="E15" s="7"/>
       <c r="F15" s="14"/>
     </row>
@@ -845,7 +854,7 @@
         <v>7</v>
       </c>
       <c r="D16" s="7"/>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="25" t="s">
         <v>16</v>
       </c>
       <c r="F16" s="14" t="s">
@@ -860,11 +869,11 @@
         <f t="shared" si="0"/>
         <v>42926</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="28" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="17"/>
-      <c r="E17" s="22"/>
+      <c r="E17" s="26"/>
       <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -875,11 +884,11 @@
         <f t="shared" si="0"/>
         <v>42933</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="20"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="25"/>
       <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -890,9 +899,9 @@
         <f t="shared" si="0"/>
         <v>42940</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
       <c r="F19" s="14"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -903,11 +912,9 @@
         <f t="shared" si="0"/>
         <v>42947</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="20"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
       <c r="F20" s="14"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -918,43 +925,317 @@
         <f t="shared" si="0"/>
         <v>42954</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
       <c r="F21" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C22" s="13"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
+      <c r="A22" s="10">
+        <v>33</v>
+      </c>
+      <c r="B22" s="11">
+        <f t="shared" si="0"/>
+        <v>42961</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C23" s="4" t="s">
+      <c r="A23" s="10">
+        <v>34</v>
+      </c>
+      <c r="B23" s="11">
+        <f t="shared" si="0"/>
+        <v>42968</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="14"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>35</v>
+      </c>
+      <c r="B24" s="11">
+        <f t="shared" si="0"/>
+        <v>42975</v>
+      </c>
+      <c r="C24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="14"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>36</v>
+      </c>
+      <c r="B25" s="11">
+        <f t="shared" si="0"/>
+        <v>42982</v>
+      </c>
+      <c r="C25" s="23"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="14"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>37</v>
+      </c>
+      <c r="B26" s="11">
+        <f t="shared" si="0"/>
+        <v>42989</v>
+      </c>
+      <c r="C26" s="23"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="14"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>38</v>
+      </c>
+      <c r="B27" s="11">
+        <f t="shared" si="0"/>
+        <v>42996</v>
+      </c>
+      <c r="C27" s="23"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="14"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>39</v>
+      </c>
+      <c r="B28" s="11">
+        <f t="shared" si="0"/>
+        <v>43003</v>
+      </c>
+      <c r="C28" s="23"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="14"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>40</v>
+      </c>
+      <c r="B29" s="11">
+        <f t="shared" si="0"/>
+        <v>43010</v>
+      </c>
+      <c r="C29" s="23"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="14"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>41</v>
+      </c>
+      <c r="B30" s="11">
+        <f t="shared" si="0"/>
+        <v>43017</v>
+      </c>
+      <c r="C30" s="23"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="14"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>42</v>
+      </c>
+      <c r="B31" s="11">
+        <f t="shared" si="0"/>
+        <v>43024</v>
+      </c>
+      <c r="C31" s="23"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="14"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>43</v>
+      </c>
+      <c r="B32" s="11">
+        <f t="shared" si="0"/>
+        <v>43031</v>
+      </c>
+      <c r="C32" s="23"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="14"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
+        <v>44</v>
+      </c>
+      <c r="B33" s="11">
+        <f t="shared" si="0"/>
+        <v>43038</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
+        <v>45</v>
+      </c>
+      <c r="B34" s="11">
+        <f t="shared" si="0"/>
+        <v>43045</v>
+      </c>
+      <c r="C34" s="21"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
+        <v>46</v>
+      </c>
+      <c r="B35" s="11">
+        <f t="shared" si="0"/>
+        <v>43052</v>
+      </c>
+      <c r="C35" s="21"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <v>47</v>
+      </c>
+      <c r="B36" s="11">
+        <f t="shared" si="0"/>
+        <v>43059</v>
+      </c>
+      <c r="C36" s="21"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
+        <v>48</v>
+      </c>
+      <c r="B37" s="11">
+        <f t="shared" si="0"/>
+        <v>43066</v>
+      </c>
+      <c r="C37" s="21"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
+        <v>49</v>
+      </c>
+      <c r="B38" s="11">
+        <f t="shared" si="0"/>
+        <v>43073</v>
+      </c>
+      <c r="C38" s="21"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="10">
+        <v>50</v>
+      </c>
+      <c r="B39" s="11">
+        <f t="shared" si="0"/>
+        <v>43080</v>
+      </c>
+      <c r="C39" s="21"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
+        <v>51</v>
+      </c>
+      <c r="B40" s="11">
+        <f t="shared" si="0"/>
+        <v>43087</v>
+      </c>
+      <c r="C40" s="21"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="10">
+        <v>52</v>
+      </c>
+      <c r="B41" s="11">
+        <f t="shared" si="0"/>
+        <v>43094</v>
+      </c>
+      <c r="C41" s="21"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C42" s="21"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C43" s="21"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C44" s="21"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C45" s="21"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C46" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="F46" s="19" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="D18:E21"/>
+    <mergeCell ref="C13:D15"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D8:E9"/>
+    <mergeCell ref="D10:D12"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="E3:E6"/>
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D8:E9"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="D20:E21"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D18:E19"/>
-    <mergeCell ref="E16:E17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C17" r:id="rId1" location="T118_F11063:8283_x405158_y123863_s15_b4"/>

</xml_diff>